<commit_message>
fix tlsf clz and ctz routines
malloc is now running quite well, free still have some bugs in it.
</commit_message>
<xml_diff>
--- a/examples/to8/boot/new-engine/memory/tlsf.xlsx
+++ b/examples/to8/boot/new-engine/memory/tlsf.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhrou\git\6809-game-builder\examples\to8\boot\new-engine\memory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF96E7AE-7493-46C1-9F65-9FBF9058B0B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46748BB4-E90D-4A4A-AA9C-8F21143B8973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="17520" xr2:uid="{CC6E1519-7F17-491B-85EE-8F6981DE1189}"/>
+    <workbookView xWindow="30420" yWindow="1785" windowWidth="26520" windowHeight="11415" xr2:uid="{CC6E1519-7F17-491B-85EE-8F6981DE1189}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="INDEX" sheetId="2" r:id="rId1"/>
+    <sheet name="Perf" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>fls</t>
   </si>
@@ -91,12 +92,33 @@
   <si>
     <t>&lt;2</t>
   </si>
+  <si>
+    <t>Minimum free size for each head of list</t>
+  </si>
+  <si>
+    <t>SL</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>1000000000000000</t>
+  </si>
+  <si>
+    <t>0100000000000000</t>
+  </si>
+  <si>
+    <t>0010000000000000</t>
+  </si>
+  <si>
+    <t>0001000000000000</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,16 +126,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -121,13 +177,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -225,7 +320,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$B$1</c:f>
+              <c:f>Perf!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -248,7 +343,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$A$2:$A$14</c:f>
+              <c:f>Perf!$A$2:$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
@@ -295,7 +390,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$2:$B$14</c:f>
+              <c:f>Perf!$B$2:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -353,7 +448,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$C$1</c:f>
+              <c:f>Perf!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -376,7 +471,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$A$2:$A$14</c:f>
+              <c:f>Perf!$A$2:$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
@@ -423,7 +518,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$C$2:$C$14</c:f>
+              <c:f>Perf!$C$2:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1571,10 +1666,1021 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C3E98D-8FD7-4E90-93C5-05DE6A2ECA88}">
+  <dimension ref="A1:S20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C2" s="5"/>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3">
+        <v>2</v>
+      </c>
+      <c r="G2" s="3">
+        <v>3</v>
+      </c>
+      <c r="H2" s="3">
+        <v>4</v>
+      </c>
+      <c r="I2" s="3">
+        <v>5</v>
+      </c>
+      <c r="J2" s="3">
+        <v>6</v>
+      </c>
+      <c r="K2" s="3">
+        <v>7</v>
+      </c>
+      <c r="L2" s="3">
+        <v>8</v>
+      </c>
+      <c r="M2" s="3">
+        <v>9</v>
+      </c>
+      <c r="N2" s="3">
+        <v>10</v>
+      </c>
+      <c r="O2" s="3">
+        <v>11</v>
+      </c>
+      <c r="P2" s="3">
+        <v>12</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>13</v>
+      </c>
+      <c r="R2" s="3">
+        <v>14</v>
+      </c>
+      <c r="S2" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="3">
+        <v>2</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="3">
+        <v>3</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>3</v>
+      </c>
+      <c r="H6" s="2">
+        <v>4</v>
+      </c>
+      <c r="I6" s="2">
+        <v>5</v>
+      </c>
+      <c r="J6" s="2">
+        <v>6</v>
+      </c>
+      <c r="K6" s="2">
+        <v>7</v>
+      </c>
+      <c r="L6" s="2">
+        <v>8</v>
+      </c>
+      <c r="M6" s="2">
+        <v>9</v>
+      </c>
+      <c r="N6" s="2">
+        <v>10</v>
+      </c>
+      <c r="O6" s="2">
+        <v>11</v>
+      </c>
+      <c r="P6" s="2">
+        <v>12</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>13</v>
+      </c>
+      <c r="R6" s="2">
+        <v>14</v>
+      </c>
+      <c r="S6" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="3">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2">
+        <v>16</v>
+      </c>
+      <c r="E7" s="2">
+        <v>17</v>
+      </c>
+      <c r="F7" s="2">
+        <v>18</v>
+      </c>
+      <c r="G7" s="2">
+        <v>19</v>
+      </c>
+      <c r="H7" s="2">
+        <v>20</v>
+      </c>
+      <c r="I7" s="2">
+        <v>21</v>
+      </c>
+      <c r="J7" s="2">
+        <v>22</v>
+      </c>
+      <c r="K7" s="2">
+        <v>23</v>
+      </c>
+      <c r="L7" s="2">
+        <v>24</v>
+      </c>
+      <c r="M7" s="2">
+        <v>25</v>
+      </c>
+      <c r="N7" s="2">
+        <v>26</v>
+      </c>
+      <c r="O7" s="2">
+        <v>27</v>
+      </c>
+      <c r="P7" s="2">
+        <v>28</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>29</v>
+      </c>
+      <c r="R7" s="2">
+        <v>30</v>
+      </c>
+      <c r="S7" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="3">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2">
+        <v>32</v>
+      </c>
+      <c r="E8" s="2">
+        <f>D8+2</f>
+        <v>34</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" ref="F8:S8" si="0">E8+2</f>
+        <v>36</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="L8" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="P8" s="2">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="Q8" s="2">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="R8" s="2">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="S8" s="2">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="3">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2">
+        <v>64</v>
+      </c>
+      <c r="E9" s="2">
+        <f>D9+4</f>
+        <v>68</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" ref="F9:S9" si="1">E9+4</f>
+        <v>72</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="L9" s="2">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="N9" s="2">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="O9" s="2">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+      <c r="P9" s="2">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="Q9" s="2">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="R9" s="2">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="S9" s="2">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="3">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2">
+        <v>128</v>
+      </c>
+      <c r="E10" s="2">
+        <f>D10+8</f>
+        <v>136</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" ref="F10:S10" si="2">E10+8</f>
+        <v>144</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="2"/>
+        <v>152</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="2"/>
+        <v>168</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="2"/>
+        <v>176</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="2"/>
+        <v>184</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" si="2"/>
+        <v>192</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="2"/>
+        <v>200</v>
+      </c>
+      <c r="N10" s="2">
+        <f t="shared" si="2"/>
+        <v>208</v>
+      </c>
+      <c r="O10" s="2">
+        <f t="shared" si="2"/>
+        <v>216</v>
+      </c>
+      <c r="P10" s="2">
+        <f t="shared" si="2"/>
+        <v>224</v>
+      </c>
+      <c r="Q10" s="2">
+        <f t="shared" si="2"/>
+        <v>232</v>
+      </c>
+      <c r="R10" s="2">
+        <f t="shared" si="2"/>
+        <v>240</v>
+      </c>
+      <c r="S10" s="2">
+        <f t="shared" si="2"/>
+        <v>248</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="3">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2">
+        <v>256</v>
+      </c>
+      <c r="E11" s="2">
+        <f>D11+16</f>
+        <v>272</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" ref="F11:S11" si="3">E11+16</f>
+        <v>288</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="3"/>
+        <v>304</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="3"/>
+        <v>320</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="3"/>
+        <v>336</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="3"/>
+        <v>352</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="3"/>
+        <v>368</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" si="3"/>
+        <v>384</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="3"/>
+        <v>400</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" si="3"/>
+        <v>416</v>
+      </c>
+      <c r="O11" s="2">
+        <f t="shared" si="3"/>
+        <v>432</v>
+      </c>
+      <c r="P11" s="2">
+        <f t="shared" si="3"/>
+        <v>448</v>
+      </c>
+      <c r="Q11" s="2">
+        <f t="shared" si="3"/>
+        <v>464</v>
+      </c>
+      <c r="R11" s="2">
+        <f t="shared" si="3"/>
+        <v>480</v>
+      </c>
+      <c r="S11" s="2">
+        <f t="shared" si="3"/>
+        <v>496</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="3">
+        <v>9</v>
+      </c>
+      <c r="D12" s="2">
+        <v>512</v>
+      </c>
+      <c r="E12" s="2">
+        <f>D12+32</f>
+        <v>544</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" ref="F12:S12" si="4">E12+32</f>
+        <v>576</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="4"/>
+        <v>608</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="4"/>
+        <v>640</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="4"/>
+        <v>672</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="4"/>
+        <v>704</v>
+      </c>
+      <c r="K12" s="2">
+        <f t="shared" si="4"/>
+        <v>736</v>
+      </c>
+      <c r="L12" s="2">
+        <f t="shared" si="4"/>
+        <v>768</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="4"/>
+        <v>800</v>
+      </c>
+      <c r="N12" s="2">
+        <f t="shared" si="4"/>
+        <v>832</v>
+      </c>
+      <c r="O12" s="2">
+        <f t="shared" si="4"/>
+        <v>864</v>
+      </c>
+      <c r="P12" s="2">
+        <f t="shared" si="4"/>
+        <v>896</v>
+      </c>
+      <c r="Q12" s="2">
+        <f t="shared" si="4"/>
+        <v>928</v>
+      </c>
+      <c r="R12" s="2">
+        <f t="shared" si="4"/>
+        <v>960</v>
+      </c>
+      <c r="S12" s="2">
+        <f t="shared" si="4"/>
+        <v>992</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="3">
+        <v>10</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1024</v>
+      </c>
+      <c r="E13" s="2">
+        <f>D13+64</f>
+        <v>1088</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" ref="F13:S13" si="5">E13+64</f>
+        <v>1152</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="5"/>
+        <v>1216</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="5"/>
+        <v>1280</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="5"/>
+        <v>1344</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="5"/>
+        <v>1408</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" si="5"/>
+        <v>1472</v>
+      </c>
+      <c r="L13" s="2">
+        <f t="shared" si="5"/>
+        <v>1536</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="5"/>
+        <v>1600</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" si="5"/>
+        <v>1664</v>
+      </c>
+      <c r="O13" s="2">
+        <f t="shared" si="5"/>
+        <v>1728</v>
+      </c>
+      <c r="P13" s="2">
+        <f t="shared" si="5"/>
+        <v>1792</v>
+      </c>
+      <c r="Q13" s="2">
+        <f t="shared" si="5"/>
+        <v>1856</v>
+      </c>
+      <c r="R13" s="2">
+        <f t="shared" si="5"/>
+        <v>1920</v>
+      </c>
+      <c r="S13" s="2">
+        <f t="shared" si="5"/>
+        <v>1984</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="3">
+        <v>11</v>
+      </c>
+      <c r="D14" s="2">
+        <v>2048</v>
+      </c>
+      <c r="E14" s="2">
+        <f>D14+128</f>
+        <v>2176</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" ref="F14:S14" si="6">E14+128</f>
+        <v>2304</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="6"/>
+        <v>2432</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="6"/>
+        <v>2560</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="6"/>
+        <v>2688</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="6"/>
+        <v>2816</v>
+      </c>
+      <c r="K14" s="2">
+        <f t="shared" si="6"/>
+        <v>2944</v>
+      </c>
+      <c r="L14" s="2">
+        <f t="shared" si="6"/>
+        <v>3072</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="6"/>
+        <v>3200</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="6"/>
+        <v>3328</v>
+      </c>
+      <c r="O14" s="2">
+        <f t="shared" si="6"/>
+        <v>3456</v>
+      </c>
+      <c r="P14" s="2">
+        <f t="shared" si="6"/>
+        <v>3584</v>
+      </c>
+      <c r="Q14" s="2">
+        <f t="shared" si="6"/>
+        <v>3712</v>
+      </c>
+      <c r="R14" s="2">
+        <f t="shared" si="6"/>
+        <v>3840</v>
+      </c>
+      <c r="S14" s="2">
+        <f t="shared" si="6"/>
+        <v>3968</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="3">
+        <v>12</v>
+      </c>
+      <c r="D15" s="2">
+        <v>4096</v>
+      </c>
+      <c r="E15" s="2">
+        <f>D15+256</f>
+        <v>4352</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" ref="F15:S15" si="7">E15+256</f>
+        <v>4608</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="7"/>
+        <v>4864</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="7"/>
+        <v>5120</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="7"/>
+        <v>5376</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="7"/>
+        <v>5632</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" si="7"/>
+        <v>5888</v>
+      </c>
+      <c r="L15" s="2">
+        <f t="shared" si="7"/>
+        <v>6144</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="7"/>
+        <v>6400</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" si="7"/>
+        <v>6656</v>
+      </c>
+      <c r="O15" s="2">
+        <f t="shared" si="7"/>
+        <v>6912</v>
+      </c>
+      <c r="P15" s="2">
+        <f t="shared" si="7"/>
+        <v>7168</v>
+      </c>
+      <c r="Q15" s="2">
+        <f t="shared" si="7"/>
+        <v>7424</v>
+      </c>
+      <c r="R15" s="2">
+        <f t="shared" si="7"/>
+        <v>7680</v>
+      </c>
+      <c r="S15" s="2">
+        <f t="shared" si="7"/>
+        <v>7936</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="3">
+        <v>13</v>
+      </c>
+      <c r="D16" s="2">
+        <v>8192</v>
+      </c>
+      <c r="E16" s="2">
+        <f>D16+512</f>
+        <v>8704</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" ref="F16:S16" si="8">E16+512</f>
+        <v>9216</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="8"/>
+        <v>9728</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="8"/>
+        <v>10240</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="8"/>
+        <v>10752</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="8"/>
+        <v>11264</v>
+      </c>
+      <c r="K16" s="2">
+        <f t="shared" si="8"/>
+        <v>11776</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" si="8"/>
+        <v>12288</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="8"/>
+        <v>12800</v>
+      </c>
+      <c r="N16" s="2">
+        <f t="shared" si="8"/>
+        <v>13312</v>
+      </c>
+      <c r="O16" s="2">
+        <f t="shared" si="8"/>
+        <v>13824</v>
+      </c>
+      <c r="P16" s="2">
+        <f t="shared" si="8"/>
+        <v>14336</v>
+      </c>
+      <c r="Q16" s="2">
+        <f t="shared" si="8"/>
+        <v>14848</v>
+      </c>
+      <c r="R16" s="2">
+        <f t="shared" si="8"/>
+        <v>15360</v>
+      </c>
+      <c r="S16" s="2">
+        <f t="shared" si="8"/>
+        <v>15872</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="3">
+        <v>14</v>
+      </c>
+      <c r="D17" s="2">
+        <v>16384</v>
+      </c>
+      <c r="E17" s="2">
+        <f>D17+1024</f>
+        <v>17408</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" ref="F17:S17" si="9">E17+1024</f>
+        <v>18432</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="9"/>
+        <v>19456</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="9"/>
+        <v>20480</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="9"/>
+        <v>21504</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" si="9"/>
+        <v>22528</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" si="9"/>
+        <v>23552</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" si="9"/>
+        <v>24576</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" si="9"/>
+        <v>25600</v>
+      </c>
+      <c r="N17" s="2">
+        <f t="shared" si="9"/>
+        <v>26624</v>
+      </c>
+      <c r="O17" s="2">
+        <f t="shared" si="9"/>
+        <v>27648</v>
+      </c>
+      <c r="P17" s="2">
+        <f t="shared" si="9"/>
+        <v>28672</v>
+      </c>
+      <c r="Q17" s="2">
+        <f t="shared" si="9"/>
+        <v>29696</v>
+      </c>
+      <c r="R17" s="2">
+        <f t="shared" si="9"/>
+        <v>30720</v>
+      </c>
+      <c r="S17" s="2">
+        <f t="shared" si="9"/>
+        <v>31744</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="3">
+        <v>15</v>
+      </c>
+      <c r="D18" s="2">
+        <v>32768</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D1:S1"/>
+    <mergeCell ref="A3:A18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F983F45-6CAC-4CB0-A119-7E01978ADF58}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>

</xml_diff>